<commit_message>
fix(ranges): Correct ranges operators!
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -339,8 +339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -501,10 +501,6 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f>SUM(G11:G12)</f>
-        <v>18</v>
-      </c>
       <c r="G12">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
test: Increment test difficulty.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16305" tabRatio="500"/>
@@ -339,8 +339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -350,7 +350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -370,7 +370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -390,7 +390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -410,7 +410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -430,7 +430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUM(B2:E5)</f>
         <v>40</v>
@@ -456,7 +456,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUM(a,b,d,e,f,g)</f>
         <v>104</v>
@@ -478,7 +478,10 @@
         <v>40</v>
       </c>
       <c r="G9">
-        <f t="array" ref="G9:G12">G2:G5+E2:E5</f>
+        <f t="array" ref="G9:H12">G2:G5+E2:E5</f>
+        <v>7</v>
+      </c>
+      <c r="H9">
         <v>7</v>
       </c>
     </row>
@@ -494,14 +497,27 @@
       <c r="G10">
         <v>7</v>
       </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f>SUM(G10:G11,G12)</f>
+        <v>25</v>
+      </c>
       <c r="G11">
         <v>9</v>
       </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
teat(excel): Complete test with Arrays.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -329,7 +329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -337,20 +337,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -370,7 +370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -390,7 +390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -416,8 +416,15 @@
       <c r="K4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="array" ref="M4:N5">{1,2;1,2}</f>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -442,14 +449,31 @@
       <c r="K5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J6" t="e">
         <f>J4:K5</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <f>{1,2;1,2}</f>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f t="array" ref="L6:M7">K6+K5</f>
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUM(B2:E5)</f>
         <v>40</v>
@@ -474,8 +498,14 @@
         <f>AVERAGE(B2:E5)</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J8">
         <f t="array" ref="J8:K10">G2:H2</f>
         <v>5</v>
@@ -484,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUM(a,b,d,e,f,g)</f>
         <v>104</v>
@@ -519,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(B2:E5)</f>
         <v>40</v>
@@ -541,7 +571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F11">
         <f>SUM(G10:G11,G12)</f>
         <v>25</v>
@@ -553,7 +583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G12">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
test: Add more tests.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16305" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,13 +23,24 @@
     <definedName name="f">Sheet1!$G$2:$H$5</definedName>
     <definedName name="g">Sheet2!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>ca</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -329,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -337,13 +354,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N12"/>
+  <dimension ref="B1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1">
@@ -589,6 +606,104 @@
       </c>
       <c r="H12">
         <v>9</v>
+      </c>
+      <c r="K12" t="e">
+        <f>J8:K10 L6:M7</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="str">
+        <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
+        <v>ciao ccca</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E14" t="str">
+        <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
+        <v>ciao ccca</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <f t="array" ref="H16:J18">G11:H12</f>
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+      <c r="H17">
+        <v>9</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f>D16*3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f>C19+1</f>
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H24" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -604,7 +719,7 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2">

</xml_diff>

<commit_message>
test: Add external links.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16305" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="a">Sheet1!$B$2:$C$3</definedName>
     <definedName name="b">Sheet1!$D$2:$E$3</definedName>
@@ -23,11 +21,8 @@
     <definedName name="f">Sheet1!$G$2:$H$5</definedName>
     <definedName name="g">Sheet2!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -89,6 +84,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -357,10 +376,10 @@
   <dimension ref="B1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1">
@@ -612,7 +631,7 @@
         <v>#NULL!</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>0</v>
       </c>
@@ -621,13 +640,13 @@
         <v>ciao ccca</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E14" t="str">
         <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
         <v>ciao ccca</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1</v>
       </c>
@@ -635,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H16">
         <f t="array" ref="H16:J18">G11:H12</f>
         <v>9</v>
@@ -647,7 +666,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>[1]Sheet1!$A$1+1</f>
+        <v>3</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="H17">
         <v>9</v>
@@ -659,7 +682,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
+        <v>4</v>
+      </c>
       <c r="H18" t="e">
         <v>#N/A</v>
       </c>
@@ -670,19 +697,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -691,17 +718,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -719,7 +746,7 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2">

</xml_diff>

<commit_message>
feat(functions): Add IFERROR function.
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -21,7 +21,7 @@
     <definedName name="f">Sheet1!$G$2:$H$5</definedName>
     <definedName name="g">Sheet2!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -376,7 +376,7 @@
   <dimension ref="B1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="L16" sqref="L16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -645,6 +645,17 @@
         <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
         <v>ciao ccca</v>
       </c>
+      <c r="K14">
+        <f>IFERROR(K12,3)</f>
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <f t="array" ref="M14:N16">IFERROR(I16:J18,1)</f>
+        <v>9</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -652,6 +663,16 @@
       </c>
       <c r="C15" s="1">
         <v>0</v>
+      </c>
+      <c r="K15">
+        <f>IFERROR(K14,1)</f>
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>9</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -664,6 +685,12 @@
       </c>
       <c r="J16" t="e">
         <v>#N/A</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>